<commit_message>
First cut of expansion, base study and identifiers
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF26F39-2772-604B-A8A7-5C61B9710616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DDEE4F-D52F-EC48-8B10-71C62E8F2E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="46980" yWindow="3240" windowWidth="28800" windowHeight="16580" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="study" sheetId="2" r:id="rId1"/>
+    <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
+    <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
+    <sheet name="soa" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -50,9 +53,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Follow Up</t>
-  </si>
-  <si>
     <t>Cycle</t>
   </si>
   <si>
@@ -138,6 +138,75 @@
   </si>
   <si>
     <t>Something Else</t>
+  </si>
+  <si>
+    <t>studyTitle</t>
+  </si>
+  <si>
+    <t>studyVersion</t>
+  </si>
+  <si>
+    <t>studyType</t>
+  </si>
+  <si>
+    <t>studyPhase</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>C98388=Interventional Study</t>
+  </si>
+  <si>
+    <t>C15602=Phase III Trial</t>
+  </si>
+  <si>
+    <t>organisationIdentifierScheme</t>
+  </si>
+  <si>
+    <t>organisationIdentifier</t>
+  </si>
+  <si>
+    <t>organisationName</t>
+  </si>
+  <si>
+    <t>organisationType</t>
+  </si>
+  <si>
+    <t>studyIdentifier</t>
+  </si>
+  <si>
+    <t>USGOV</t>
+  </si>
+  <si>
+    <t>CT-GOV</t>
+  </si>
+  <si>
+    <t>ClinicalTrials.gov</t>
+  </si>
+  <si>
+    <t>Registry</t>
+  </si>
+  <si>
+    <t>NCT12345678</t>
+  </si>
+  <si>
+    <t>Simple Test 1</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screening </t>
+  </si>
+  <si>
+    <t>Follow-Up</t>
   </si>
 </sst>
 </file>
@@ -193,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -210,14 +279,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,14 +606,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="4" width="30.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="5" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,10 +806,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="7"/>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
@@ -562,278 +817,278 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5" t="s">
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5" t="s">
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add simple address handling
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F464FD9-BD48-BB4D-AE3B-D55E51B81516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D6D739-F42E-6C44-A3A8-03D972B8A3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="2840" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -207,13 +207,49 @@
   </si>
   <si>
     <t>Follow-Up</t>
+  </si>
+  <si>
+    <t>therapeuticAreas</t>
+  </si>
+  <si>
+    <t>studyDesignRationale</t>
+  </si>
+  <si>
+    <t>studyDesignBlindingScheme</t>
+  </si>
+  <si>
+    <t>"Study design rationale put here"</t>
+  </si>
+  <si>
+    <t>C49659=OPEN LABEL</t>
+  </si>
+  <si>
+    <t>trialIntentTypes</t>
+  </si>
+  <si>
+    <t>interventionModel</t>
+  </si>
+  <si>
+    <t>C12345=Observational</t>
+  </si>
+  <si>
+    <t>C12346=None</t>
+  </si>
+  <si>
+    <t>trialTypes</t>
+  </si>
+  <si>
+    <t>C15714=BASIC SCIENCE, C139174=DEVICE FEASIBILITY</t>
+  </si>
+  <si>
+    <t>Not supported yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +267,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -262,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -292,6 +336,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,79 +765,153 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -790,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>

</xml_diff>

<commit_message>
Refactor BCs in Activities
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAE4386-B7F1-784F-8C83-F7937868E0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F8186-0049-7F43-83E5-609A3E5135AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="-160" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -128,15 +128,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>BC:Age</t>
-  </si>
-  <si>
-    <t>BC:Sex</t>
-  </si>
-  <si>
-    <t>BC:Race</t>
-  </si>
-  <si>
     <t>Something Else</t>
   </si>
   <si>
@@ -243,6 +234,9 @@
   </si>
   <si>
     <t>Not supported yet</t>
+  </si>
+  <si>
+    <t>BC:Age, BC:Sex, BC:Race</t>
   </si>
 </sst>
 </file>
@@ -331,23 +325,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,30 +671,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -712,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -726,36 +720,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -779,73 +773,73 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+        <v>53</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+        <v>54</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+        <v>62</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>14</v>
@@ -854,41 +848,41 @@
         <v>3</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>52</v>
+      <c r="A9" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>53</v>
+      <c r="A10" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -905,12 +899,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -918,28 +912,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
-    <col min="4" max="10" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="19.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
+    <col min="4" max="8" width="12.33203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
@@ -949,17 +944,17 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
@@ -980,8 +975,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1002,8 +997,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1024,8 +1019,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1046,8 +1041,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
@@ -1068,8 +1063,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1090,8 +1085,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1125,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -1147,77 +1142,25 @@
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>30</v>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix activity cross ref
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F8186-0049-7F43-83E5-609A3E5135AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92224BCC-0105-0040-AF7C-BC7A265D375E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -329,13 +329,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -775,67 +775,67 @@
       <c r="A1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
@@ -918,7 +918,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Roche example, allow all to be run in one go
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92224BCC-0105-0040-AF7C-BC7A265D375E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA80F711-1BB1-FE42-8976-EB16DEBDA534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -660,7 +660,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,7 +707,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,7 +762,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E10" sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add address, initial cut
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA80F711-1BB1-FE42-8976-EB16DEBDA534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A422C516-063E-B74B-BCDD-5948DB3C377A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="37680" yWindow="7420" windowWidth="28800" windowHeight="16580" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>BC:Age, BC:Sex, BC:Race</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>line|city|district|state|postal_code|GBR</t>
   </si>
 </sst>
 </file>
@@ -704,10 +710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,9 +722,10 @@
     <col min="2" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
@@ -734,8 +741,11 @@
       <c r="E1" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -750,6 +760,9 @@
       </c>
       <c r="E2" t="s">
         <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -914,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>

</xml_diff>

<commit_message>
First cut interventions and indications
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D508B05-8A7C-B642-92F4-BBBFC6B0A270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96394C9-DDD2-D042-86FF-F9E4B684FECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67680" yWindow="1060" windowWidth="28800" windowHeight="16580" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="34260" yWindow="3080" windowWidth="28800" windowHeight="16580" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
     <sheet name="soa" sheetId="1" r:id="rId4"/>
+    <sheet name="indications_interventions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -261,6 +262,39 @@
   </si>
   <si>
     <t>C15602</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>codes</t>
+  </si>
+  <si>
+    <t>An indication</t>
+  </si>
+  <si>
+    <t>SNOMED:12345=Indication1</t>
+  </si>
+  <si>
+    <t>An intervention</t>
+  </si>
+  <si>
+    <t>ICD-10: X = Y, SNOMED: A=B</t>
+  </si>
+  <si>
+    <t>SNOMED:345678=Indication2</t>
+  </si>
+  <si>
+    <t>ICD-10: DD=CC, SNOMED: A=B</t>
   </si>
 </sst>
 </file>
@@ -692,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1232,4 +1266,78 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Study Populations, first cut
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB497D8-8A84-DD4F-B82A-15FEF5736C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAC70FC-A625-D945-BFB2-380643E4EC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34260" yWindow="3080" windowWidth="28800" windowHeight="16580" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="64580" yWindow="500" windowWidth="33800" windowHeight="16580" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
     <sheet name="soa" sheetId="1" r:id="rId4"/>
     <sheet name="indications_interventions" sheetId="6" r:id="rId5"/>
+    <sheet name="studyDesignPopulation" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="100">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -295,6 +296,51 @@
   </si>
   <si>
     <t>ICD-10: DD=CC, SNOMED: A=B</t>
+  </si>
+  <si>
+    <t>populationDescription</t>
+  </si>
+  <si>
+    <t>Pop 1</t>
+  </si>
+  <si>
+    <t>plannedNumberOfParticipants</t>
+  </si>
+  <si>
+    <t>plannedMinimumAgeOfParticipants</t>
+  </si>
+  <si>
+    <t>18 years</t>
+  </si>
+  <si>
+    <t>40 years</t>
+  </si>
+  <si>
+    <t>plannedSexOfParticipants</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>Pop 2</t>
+  </si>
+  <si>
+    <t>60 years</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Pop 3</t>
+  </si>
+  <si>
+    <t>70 years</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>plannedMaximumAgeOfParticipants</t>
   </si>
 </sst>
 </file>
@@ -1272,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,4 +1386,96 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add in configuration of CT versions
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1CBF75-F70D-7648-8FF8-453A4DE8C6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB56AAE7-C205-6B4E-A001-051B815FE79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72240" yWindow="500" windowWidth="28160" windowHeight="26800" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="72240" yWindow="500" windowWidth="28160" windowHeight="26800" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="studyDesignPopulations" sheetId="7" r:id="rId6"/>
     <sheet name="studyDesignOE" sheetId="8" r:id="rId7"/>
     <sheet name="studyDesignEstimands" sheetId="9" r:id="rId8"/>
+    <sheet name="configuration" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="179">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -571,6 +572,15 @@
   </si>
   <si>
     <t>Efficacy Study</t>
+  </si>
+  <si>
+    <t>CT Version</t>
+  </si>
+  <si>
+    <t>SPONSOR =   12</t>
+  </si>
+  <si>
+    <t>SNOMED=January 31, 2018</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2485,4 +2495,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First cut of better Estimands
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D64CE9-31FF-D041-ACF8-6399B074F826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7F3607-ADB3-3F47-99F2-E20B59EBF8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72240" yWindow="500" windowWidth="28160" windowHeight="26800" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="59820" yWindow="500" windowWidth="40580" windowHeight="26800" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="186">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -581,6 +581,27 @@
   </si>
   <si>
     <t>SNOMED=January 31, 2018</t>
+  </si>
+  <si>
+    <t>A second bad event</t>
+  </si>
+  <si>
+    <t>A third bad thing</t>
+  </si>
+  <si>
+    <t>EST2</t>
+  </si>
+  <si>
+    <t>Something else</t>
+  </si>
+  <si>
+    <t>Bad stuff</t>
+  </si>
+  <si>
+    <t>IC Event Description Number 2</t>
+  </si>
+  <si>
+    <t>Really really bad shit</t>
   </si>
 </sst>
 </file>
@@ -2424,10 +2445,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2436,8 +2457,8 @@
     <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
-    <col min="7" max="8" width="17" customWidth="1"/>
+    <col min="6" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -2457,13 +2478,13 @@
         <v>149</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>142</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2483,13 +2504,49 @@
         <v>150</v>
       </c>
       <c r="F2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" t="s">
         <v>147</v>
       </c>
-      <c r="G2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" t="s">
-        <v>128</v>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2501,7 +2558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Variable name for main SoA (timeline) sheet
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EE9F6D-1C2A-8B41-97F9-371D8C96A32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964E8ED5-E15F-FF4C-BD62-620DBBC33CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="59820" yWindow="500" windowWidth="40580" windowHeight="26800" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -16,12 +16,13 @@
     <sheet name="study" sheetId="2" r:id="rId1"/>
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
-    <sheet name="soa" sheetId="1" r:id="rId4"/>
-    <sheet name="studyDesignII" sheetId="6" r:id="rId5"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId6"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId7"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId8"/>
-    <sheet name="configuration" sheetId="10" r:id="rId9"/>
+    <sheet name="mainTimeline" sheetId="1" r:id="rId4"/>
+    <sheet name="profileTimeline" sheetId="11" r:id="rId5"/>
+    <sheet name="studyDesignII" sheetId="6" r:id="rId6"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId7"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId8"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId9"/>
+    <sheet name="configuration" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="189">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -602,6 +603,15 @@
   </si>
   <si>
     <t>SPONSOR:T2_DIABETES=Type 2 diabetes, SNOMED: 73211009=Diabetes mellitus (disorder)</t>
+  </si>
+  <si>
+    <t>mainTimeline</t>
+  </si>
+  <si>
+    <t>otherTimelines</t>
+  </si>
+  <si>
+    <t>profileTimeline</t>
   </si>
 </sst>
 </file>
@@ -736,14 +746,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1345,6 +1355,40 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:F3"/>
@@ -1429,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,12 +1490,12 @@
       <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -1508,68 +1552,92 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
@@ -1602,10 +1670,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1615,17 +1683,17 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1646,8 +1714,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1668,8 +1736,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1690,8 +1758,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1712,8 +1780,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
@@ -1734,8 +1802,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1756,8 +1824,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1846,6 +1914,269 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE8670E-14F5-DF47-B190-1E715EB319D4}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
+    <col min="4" max="8" width="12.33203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B8"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1934,7 +2265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -2026,7 +2357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -2436,7 +2767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -2545,38 +2876,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update simple example for Study Design Rationale
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA0C684-3891-DC4D-8C67-324E1C83819F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E106106-40FD-B646-8707-FE726628B43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="39900" yWindow="800" windowWidth="33600" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -203,9 +203,6 @@
     <t>studyDesignBlindingScheme</t>
   </si>
   <si>
-    <t>"Study design rationale put here"</t>
-  </si>
-  <si>
     <t>trialIntentTypes</t>
   </si>
   <si>
@@ -657,6 +654,9 @@
   </si>
   <si>
     <t>Only do it they have man flu</t>
+  </si>
+  <si>
+    <t>Basic study</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1179,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1193,7 +1193,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -1204,10 +1204,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1218,10 +1218,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>166</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>167</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1256,42 +1256,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="F9" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>157</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>162</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1301,33 +1301,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>161</v>
-      </c>
       <c r="D11" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G11" s="20">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1430,18 +1430,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" t="s">
         <v>172</v>
-      </c>
-      <c r="B2" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1483,7 +1483,7 @@
         <v>38</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1497,33 +1497,33 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1535,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1551,7 +1551,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -1562,7 +1562,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>52</v>
+        <v>203</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -1573,7 +1573,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -1592,10 +1592,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -1603,10 +1603,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
@@ -1729,10 +1729,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>187</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>188</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -1753,10 +1753,10 @@
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>189</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>190</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -1779,10 +1779,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>191</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>192</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
@@ -1927,7 +1927,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -1996,72 +1996,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2088,72 +2088,72 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
         <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
         <v>89</v>
-      </c>
-      <c r="E4" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2180,205 +2180,205 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>103</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2591,90 +2591,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>137</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
         <v>140</v>
       </c>
-      <c r="B2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>141</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
         <v>142</v>
-      </c>
-      <c r="E2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
         <v>177</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
         <v>178</v>
       </c>
-      <c r="C5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>179</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" t="s">
         <v>180</v>
-      </c>
-      <c r="F5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H5" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2702,47 +2702,47 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>195</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
         <v>197</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>198</v>
-      </c>
-      <c r="C2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
         <v>200</v>
       </c>
-      <c r="B3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" t="s">
         <v>202</v>
-      </c>
-      <c r="E3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
First cut of separating Encounters
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E106106-40FD-B646-8707-FE726628B43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37D1D7A-35EE-B24D-9F5C-07B8880DB9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39900" yWindow="800" windowWidth="33600" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="68340" yWindow="2520" windowWidth="33260" windowHeight="19480" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="studyDesignOE" sheetId="8" r:id="rId7"/>
     <sheet name="studyDesignEstimands" sheetId="9" r:id="rId8"/>
     <sheet name="studyDesignProcedures" sheetId="11" r:id="rId9"/>
-    <sheet name="configuration" sheetId="10" r:id="rId10"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId10"/>
+    <sheet name="configuration" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="230">
   <si>
     <t>Epoch</t>
   </si>
@@ -62,15 +63,9 @@
     <t>Cycle End Rule</t>
   </si>
   <si>
-    <t>Visit Label</t>
-  </si>
-  <si>
     <t>A:</t>
   </si>
   <si>
-    <t>Visit Window</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -125,9 +120,6 @@
     <t>Timing</t>
   </si>
   <si>
-    <t>BC/Profile</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -657,6 +649,93 @@
   </si>
   <si>
     <t>Basic study</t>
+  </si>
+  <si>
+    <t>encounterName</t>
+  </si>
+  <si>
+    <t>encounterDescription</t>
+  </si>
+  <si>
+    <t>encounterType</t>
+  </si>
+  <si>
+    <t>encounterEnvironmentalSetting</t>
+  </si>
+  <si>
+    <t>encounterContactModes</t>
+  </si>
+  <si>
+    <t>transitionStartRule</t>
+  </si>
+  <si>
+    <t>transitionEndRule</t>
+  </si>
+  <si>
+    <t>Screening encounter</t>
+  </si>
+  <si>
+    <t>Baseline encounter</t>
+  </si>
+  <si>
+    <t>First dose</t>
+  </si>
+  <si>
+    <t>2 week visit</t>
+  </si>
+  <si>
+    <t>5 week visit</t>
+  </si>
+  <si>
+    <t>Visit</t>
+  </si>
+  <si>
+    <t>CLINIC</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>In Person</t>
+  </si>
+  <si>
+    <t>TELEPHONE CALL</t>
+  </si>
+  <si>
+    <t>Subject identifier</t>
+  </si>
+  <si>
+    <t>IEs passed</t>
+  </si>
+  <si>
+    <t>Radomized</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>Encounter xref</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>BC/Procedure/Timeline</t>
+  </si>
+  <si>
+    <t>Epoch/Arms</t>
   </si>
 </sst>
 </file>
@@ -739,12 +818,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -756,7 +829,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -770,14 +842,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -785,17 +851,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -814,6 +871,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1132,7 +1209,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,271 +1217,271 @@
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="16" style="9" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="17" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="17" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="A1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="A3" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="A6" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="A7" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="E9" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="F9" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="G9" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="H9" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="19" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="B10" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="C10" s="11" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>161</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="20">
+      <c r="G10" s="15">
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="A11" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>160</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>163</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G11" s="20">
+        <v>161</v>
+      </c>
+      <c r="G11" s="15">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1416,6 +1493,165 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="3" customWidth="1"/>
+    <col min="6" max="8" width="27.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1429,19 +1665,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>171</v>
+      <c r="A1" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>171</v>
+      <c r="A2" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1454,7 +1690,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1467,63 +1703,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="E1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>61</v>
+      <c r="F1" s="27" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="F3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1535,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1547,150 +1783,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="B4" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="B6" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="A7" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
+      <c r="A8" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="A10" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>48</v>
+      <c r="E10" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>44</v>
+      <c r="A11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>44</v>
+      <c r="A12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1711,11 +1950,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1728,247 +1967,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="17" t="s">
+        <v>226</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>221</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>222</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>26</v>
+      <c r="A9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1995,73 +2234,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>69</v>
+      <c r="D1" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
-      </c>
-      <c r="D5" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2087,73 +2326,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
         <v>80</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>88</v>
+        <v>77</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2179,391 +2418,391 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="B3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="E3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E8" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E10" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E11" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E13" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2590,91 +2829,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>137</v>
+      <c r="G1" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" t="s">
         <v>139</v>
-      </c>
-      <c r="B2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" t="s">
         <v>176</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" t="s">
         <v>177</v>
-      </c>
-      <c r="C5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2695,58 +2934,58 @@
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24" style="9" customWidth="1"/>
+    <col min="4" max="4" width="24" style="7" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>192</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" t="s">
         <v>199</v>
       </c>
-      <c r="B3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
+      <c r="B5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small tweak, spelling mistake
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37D1D7A-35EE-B24D-9F5C-07B8880DB9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DC6F08-62E6-6F4C-B890-6FFB31FC2BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68340" yWindow="2520" windowWidth="33260" windowHeight="19480" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="68340" yWindow="2520" windowWidth="33260" windowHeight="19480" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -702,9 +702,6 @@
     <t>TELEPHONE CALL</t>
   </si>
   <si>
-    <t>Subject identifier</t>
-  </si>
-  <si>
     <t>IEs passed</t>
   </si>
   <si>
@@ -736,6 +733,9 @@
   </si>
   <si>
     <t>Epoch/Arms</t>
+  </si>
+  <si>
+    <t>Subject identified</t>
   </si>
 </sst>
 </file>
@@ -807,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -860,6 +860,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -871,26 +882,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,7 +1215,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -1238,7 +1229,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1252,7 +1243,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="20" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1266,7 +1257,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1280,7 +1271,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="20" t="s">
         <v>143</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -1294,7 +1285,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="20" t="s">
         <v>144</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1308,7 +1299,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="20" t="s">
         <v>162</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1332,28 +1323,28 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="21" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1496,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,34 +1502,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="24" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1556,15 +1547,15 @@
         <v>216</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -1584,7 +1575,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -1602,12 +1593,12 @@
         <v>216</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
@@ -1627,7 +1618,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
@@ -1703,22 +1694,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="23" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1786,91 +1777,91 @@
       <c r="A1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>44</v>
@@ -1950,7 +1941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -1970,7 +1961,7 @@
       <c r="A1" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="11" t="s">
         <v>184</v>
       </c>
       <c r="C1" s="17" t="s">
@@ -1982,10 +1973,10 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1994,7 +1985,7 @@
       <c r="A2" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="16" t="s">
         <v>186</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -2020,7 +2011,7 @@
       <c r="A3" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="3" t="s">
         <v>188</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -2043,8 +2034,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="17" t="s">
         <v>22</v>
       </c>
@@ -2065,8 +2056,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="17" t="s">
         <v>4</v>
       </c>
@@ -2087,8 +2078,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="17" t="s">
         <v>23</v>
       </c>
@@ -2109,32 +2100,32 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="17" t="s">
         <v>226</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="17" t="s">
-        <v>227</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -2148,14 +2139,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>228</v>
+      <c r="C9" s="24" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
First cut update for study design name and description
</commit_message>
<xml_diff>
--- a/source_data/simple_1.xlsx
+++ b/source_data/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6438F0-6A53-684B-AB7A-66DA03E4514D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966D1362-35DA-C543-A9E9-98B697A8C324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68340" yWindow="2520" windowWidth="33260" windowHeight="19480" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="68320" yWindow="2520" windowWidth="33260" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="256">
   <si>
     <t>Epoch</t>
   </si>
@@ -803,6 +803,18 @@
   </si>
   <si>
     <t>Completed treatment 2</t>
+  </si>
+  <si>
+    <t>The main design for the study</t>
+  </si>
+  <si>
+    <t>Study Design 1</t>
+  </si>
+  <si>
+    <t>studyDesignName</t>
+  </si>
+  <si>
+    <t>studyDesignDescription</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1951,10 +1963,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1964,67 +1976,67 @@
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+        <v>254</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+        <v>45</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+        <v>46</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+        <v>47</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -2032,10 +2044,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>180</v>
+        <v>50</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
@@ -2043,86 +2055,110 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="26"/>
+        <v>49</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>165</v>
+      </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>